<commit_message>
Add Problems to Misc 	- EucledianGCD and LCM 	- BinaryEponentiation
	from cp-algorithms
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1738,11 +1738,11 @@
   </sheetPr>
   <dimension ref="A1:H481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A272" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A204" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C104" activeCellId="0" sqref="C104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -2843,7 +2843,7 @@
       <c r="B104" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C104" s="6" t="s">
+      <c r="C104" s="9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>